<commit_message>
adding all files ahead of merge into main
</commit_message>
<xml_diff>
--- a/data/6_tables/tables_appendix/App_Table4_scc76.xlsx
+++ b/data/6_tables/tables_appendix/App_Table4_scc76.xlsx
@@ -1872,7 +1872,7 @@
         <v>0.015305735569137965</v>
       </c>
       <c r="F19" s="1">
-        <v>0.027581443394213336</v>
+        <v>0.036535702231583637</v>
       </c>
       <c r="G19" s="1">
         <v>0.42256070921818417</v>
@@ -1881,7 +1881,7 @@
         <v>-0.041382700204849243</v>
       </c>
       <c r="I19" s="1">
-        <v>1.4434055093784621</v>
+        <v>1.4523597682158318</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
@@ -1890,13 +1890,13 @@
         <v>0.089584887027740479</v>
       </c>
       <c r="L19" s="1">
-        <v>-0.0016155967950731668</v>
+        <v>-0.0017904652279344664</v>
       </c>
       <c r="M19" s="1">
-        <v>1.0879692905156582</v>
+        <v>1.0877944220827975</v>
       </c>
       <c r="N19" s="1">
-        <v>1.3266968727111816</v>
+        <v>1.3351417779922485</v>
       </c>
     </row>
     <row r="20">
@@ -1916,7 +1916,7 @@
         <v>0.018366737671729898</v>
       </c>
       <c r="F20" s="1">
-        <v>0.038592122496077803</v>
+        <v>0.051355386798866101</v>
       </c>
       <c r="G20" s="1">
         <v>0.52689957618713379</v>
@@ -1925,7 +1925,7 @@
         <v>-0.049658849835395813</v>
       </c>
       <c r="I20" s="1">
-        <v>1.5574077906275141</v>
+        <v>1.5701710549303021</v>
       </c>
       <c r="J20" s="1">
         <v>1</v>
@@ -1934,13 +1934,13 @@
         <v>0.10607463866472244</v>
       </c>
       <c r="L20" s="1">
-        <v>-0.0020233809530395002</v>
+        <v>-0.0022726357565200999</v>
       </c>
       <c r="M20" s="1">
-        <v>1.1040512593495151</v>
+        <v>1.1038020045460351</v>
       </c>
       <c r="N20" s="1">
-        <v>1.4106299661712329</v>
+        <v>1.4225115088245131</v>
       </c>
     </row>
     <row r="21">
@@ -1960,7 +1960,7 @@
         <v>0.016363903863386299</v>
       </c>
       <c r="F21" s="1">
-        <v>0.029223164338572</v>
+        <v>0.0386723777590878</v>
       </c>
       <c r="G21" s="1">
         <v>0.45102795958518982</v>
@@ -1969,7 +1969,7 @@
         <v>-0.044243711978197098</v>
       </c>
       <c r="I21" s="1">
-        <v>1.4730487401020831</v>
+        <v>1.482497953522598</v>
       </c>
       <c r="J21" s="1">
         <v>1</v>
@@ -1978,13 +1978,13 @@
         <v>0.09450753778219223</v>
       </c>
       <c r="L21" s="1">
-        <v>-0.0017232646858383999</v>
+        <v>-0.0019077991261118</v>
       </c>
       <c r="M21" s="1">
-        <v>1.092784276461549</v>
+        <v>1.0925997420212761</v>
       </c>
       <c r="N21" s="1">
-        <v>1.3479776126280261</v>
+        <v>1.356853655099737</v>
       </c>
     </row>
     <row r="22">
@@ -2004,7 +2004,7 @@
         <v>0.011186565172297699</v>
       </c>
       <c r="F22" s="1">
-        <v>0.0149290433479902</v>
+        <v>0.019579342136797</v>
       </c>
       <c r="G22" s="1">
         <v>0.28975459188222891</v>
@@ -2013,7 +2013,7 @@
         <v>-0.030245544388890266</v>
       </c>
       <c r="I22" s="1">
-        <v>1.299759997405789</v>
+        <v>1.3044102961945949</v>
       </c>
       <c r="J22" s="1">
         <v>1</v>
@@ -2022,13 +2022,13 @@
         <v>0.068172477185726166</v>
       </c>
       <c r="L22" s="1">
-        <v>-0.0011001447463416</v>
+        <v>-0.0011909608011715</v>
       </c>
       <c r="M22" s="1">
-        <v>1.0670723357359111</v>
+        <v>1.066981519681081</v>
       </c>
       <c r="N22" s="1">
-        <v>1.218061750714776</v>
+        <v>1.2225237945868841</v>
       </c>
     </row>
     <row r="23">
@@ -2048,7 +2048,7 @@
         <v>-0.0128851149359057</v>
       </c>
       <c r="F23" s="1">
-        <v>3.0181024750800001e-09</v>
+        <v>3.8113778133000003e-09</v>
       </c>
       <c r="G23" s="1">
         <v>0.00012861509458160001</v>
@@ -2057,7 +2057,7 @@
         <v>0.034837979823350906</v>
       </c>
       <c r="I23" s="1">
-        <v>1.005799853053295</v>
+        <v>1.00579985384657</v>
       </c>
       <c r="J23" s="1">
         <v>1</v>
@@ -2066,13 +2066,13 @@
         <v>-0.074416257441043854</v>
       </c>
       <c r="L23" s="1">
-        <v>0.0010000571813864999</v>
+        <v>0.0010000571658944999</v>
       </c>
       <c r="M23" s="1">
-        <v>0.92658379684643111</v>
+        <v>0.92658379683093905</v>
       </c>
       <c r="N23" s="1">
-        <v>1.0854925981616239</v>
+        <v>1.0854925990359019</v>
       </c>
     </row>
     <row r="24">
@@ -2655,40 +2655,40 @@
         <v>1</v>
       </c>
       <c r="C37" s="1">
-        <v>0.012205494819587832</v>
+        <v>0.012112803199989699</v>
       </c>
       <c r="D37" s="1">
-        <v>0.0029898660466978998</v>
+        <v>0.0029671581970759663</v>
       </c>
       <c r="E37" s="1">
-        <v>-0.021128674117923501</v>
+        <v>-0.020956450500775367</v>
       </c>
       <c r="F37" s="1">
-        <v>-7.1369847073093323e-05</v>
+        <v>-6.9413469971819986e-05</v>
       </c>
       <c r="G37" s="1">
-        <v>0.013228093545573466</v>
+        <v>0.013016943664600433</v>
       </c>
       <c r="H37" s="1">
-        <v>-0.006267232820391655</v>
+        <v>-0.0062195952050387859</v>
       </c>
       <c r="I37" s="1">
-        <v>1.000956177492198</v>
+        <v>1.0008514460091893</v>
       </c>
       <c r="J37" s="1">
         <v>1</v>
       </c>
       <c r="K37" s="1">
-        <v>0.0043544336222112179</v>
+        <v>0.004321330226957798</v>
       </c>
       <c r="L37" s="1">
-        <v>-0.00030771615731246669</v>
+        <v>-0.00030528901773486673</v>
       </c>
       <c r="M37" s="1">
-        <v>1.0040467173636214</v>
+        <v>1.0040160409828407</v>
       </c>
       <c r="N37" s="1">
-        <v>0.99692189693450928</v>
+        <v>0.99684804677963257</v>
       </c>
     </row>
     <row r="38">
@@ -2699,40 +2699,40 @@
         <v>1</v>
       </c>
       <c r="C38" s="1">
-        <v>0.0271393414643454</v>
+        <v>0.026933238430234399</v>
       </c>
       <c r="D38" s="1">
-        <v>0.0066480709527453998</v>
+        <v>0.0065975792607725998</v>
       </c>
       <c r="E38" s="1">
-        <v>-0.0469803404164294</v>
+        <v>-0.046597395224688198</v>
       </c>
       <c r="F38" s="1">
-        <v>-0.00019736115851499999</v>
+        <v>-0.00019194731806849999</v>
       </c>
       <c r="G38" s="1">
-        <v>0.029539255425334001</v>
+        <v>0.029065784066915502</v>
       </c>
       <c r="H38" s="1">
-        <v>-0.013935410417616367</v>
+        <v>-0.013829485513269901</v>
       </c>
       <c r="I38" s="1">
-        <v>1.0022135562159129</v>
+        <v>1.001977773627893</v>
       </c>
       <c r="J38" s="1">
         <v>1</v>
       </c>
       <c r="K38" s="1">
-        <v>0.0096822343766689301</v>
+        <v>0.0096086272969841957</v>
       </c>
       <c r="L38" s="1">
-        <v>-0.00068729225637680004</v>
+        <v>-0.00068182281009570005</v>
       </c>
       <c r="M38" s="1">
-        <v>1.008994941848443</v>
+        <v>1.0089268044679669</v>
       </c>
       <c r="N38" s="1">
-        <v>0.99327906875320227</v>
+        <v>0.99311245294574335</v>
       </c>
     </row>
     <row r="39">
@@ -2743,40 +2743,40 @@
         <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>0.0077885097862839996</v>
+        <v>0.0077293618699516</v>
       </c>
       <c r="D39" s="1">
-        <v>0.0019078784849438</v>
+        <v>0.0018933882646267001</v>
       </c>
       <c r="E39" s="1">
-        <v>-0.013482524680159501</v>
+        <v>-0.0133726262002143</v>
       </c>
       <c r="F39" s="1">
-        <v>-1.5999980326000001e-05</v>
+        <v>-1.55649797537e-05</v>
       </c>
       <c r="G39" s="1">
-        <v>0.0083447089418769004</v>
+        <v>0.0082130068913101994</v>
       </c>
       <c r="H39" s="1">
-        <v>-0.0039992155507206917</v>
+        <v>-0.0039688171818852425</v>
       </c>
       <c r="I39" s="1">
-        <v>1.0005433569598201</v>
+        <v>1.0004787486962039</v>
       </c>
       <c r="J39" s="1">
         <v>1</v>
       </c>
       <c r="K39" s="1">
-        <v>0.0027786295395344496</v>
+        <v>0.0027575057465583086</v>
       </c>
       <c r="L39" s="1">
-        <v>-0.00019400924032180001</v>
+        <v>-0.00019251597943310001</v>
       </c>
       <c r="M39" s="1">
-        <v>1.0025846202698141</v>
+        <v>1.0025649896765621</v>
       </c>
       <c r="N39" s="1">
-        <v>0.99796399897951294</v>
+        <v>0.99791909651559729</v>
       </c>
     </row>
     <row r="40">
@@ -2787,40 +2787,40 @@
         <v>1</v>
       </c>
       <c r="C40" s="1">
-        <v>0.0016886332081340999</v>
+        <v>0.0016758092997830999</v>
       </c>
       <c r="D40" s="1">
-        <v>0.00041364870240449998</v>
+        <v>0.00041050706582860001</v>
       </c>
       <c r="E40" s="1">
-        <v>-0.0029231572571815998</v>
+        <v>-0.0028993300774236</v>
       </c>
       <c r="F40" s="1">
-        <v>-7.4840237828000003e-07</v>
+        <v>-7.2811209326000004e-07</v>
       </c>
       <c r="G40" s="1">
-        <v>0.0018003162695094999</v>
+        <v>0.0017720400355756001</v>
       </c>
       <c r="H40" s="1">
-        <v>-0.00086707319132983685</v>
+        <v>-0.00086048251250758767</v>
       </c>
       <c r="I40" s="1">
-        <v>1.000111619300861</v>
+        <v>1.000097815703471</v>
       </c>
       <c r="J40" s="1">
         <v>1</v>
       </c>
       <c r="K40" s="1">
-        <v>0.00060243695043027401</v>
+        <v>0.00059785705525428057</v>
       </c>
       <c r="L40" s="1">
-        <v>-4.18469752388e-05</v>
+        <v>-4.1528263675799998e-05</v>
       </c>
       <c r="M40" s="1">
-        <v>1.0005605899726071</v>
+        <v>1.0005563288039929</v>
       </c>
       <c r="N40" s="1">
-        <v>0.99955128087569556</v>
+        <v>0.9995417418416912</v>
       </c>
     </row>
     <row r="41">
@@ -2831,13 +2831,13 @@
         <v>0.77409690618515015</v>
       </c>
       <c r="C41" s="1">
-        <v>0.11706141859109694</v>
+        <v>0.11819606655250758</v>
       </c>
       <c r="D41" s="1">
         <v>0.028383977662391712</v>
       </c>
       <c r="E41" s="1">
-        <v>-0.025890021623491348</v>
+        <v>-0.026112260611837468</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -2849,7 +2849,7 @@
         <v>-0.051298871636390686</v>
       </c>
       <c r="I41" s="1">
-        <v>0.84235341380941497</v>
+        <v>0.84326582278247941</v>
       </c>
       <c r="J41" s="1">
         <v>0.99999999506716952</v>
@@ -2858,13 +2858,13 @@
         <v>0.015742333605885506</v>
       </c>
       <c r="L41" s="1">
-        <v>-0.0018890645377775506</v>
+        <v>-0.0019068830451656198</v>
       </c>
       <c r="M41" s="1">
-        <v>1.0138532628993355</v>
+        <v>1.0138354443919473</v>
       </c>
       <c r="N41" s="1">
-        <v>0.83084350824356079</v>
+        <v>0.83175808191299439</v>
       </c>
     </row>
     <row r="42">
@@ -2919,13 +2919,13 @@
         <v>0.75</v>
       </c>
       <c r="C43" s="1">
-        <v>0.1542968425301729</v>
+        <v>0.15997008233722612</v>
       </c>
       <c r="D43" s="1">
         <v>0.018621671611309454</v>
       </c>
       <c r="E43" s="1">
-        <v>-0.026940264448648669</v>
+        <v>-0.028051459390379275</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
@@ -2937,7 +2937,7 @@
         <v>-0.10307729244232178</v>
       </c>
       <c r="I43" s="1">
-        <v>0.79290093316968524</v>
+        <v>0.79746297803500787</v>
       </c>
       <c r="J43" s="1">
         <v>0.99999996999575602</v>
@@ -2946,13 +2946,13 @@
         <v>0.023750618100166321</v>
       </c>
       <c r="L43" s="1">
-        <v>-0.0025583861840863908</v>
+        <v>-0.002647478721026737</v>
       </c>
       <c r="M43" s="1">
-        <v>1.0211922005423115</v>
+        <v>1.0211031080053707</v>
       </c>
       <c r="N43" s="1">
-        <v>0.77644632689968596</v>
+        <v>0.78098183404100785</v>
       </c>
     </row>
     <row r="44">
@@ -3808,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G63" s="1">
         <v>-0.0017523671022848001</v>
@@ -3817,7 +3817,7 @@
         <v>0.05981777235865593</v>
       </c>
       <c r="I63" s="1">
-        <v>0.76082820238442839</v>
+        <v>0.76082820236705972</v>
       </c>
       <c r="J63" s="1">
         <v>1</v>
@@ -3826,10 +3826,10 @@
         <v>-0.073525190353393555</v>
       </c>
       <c r="L63" s="1">
-        <v>0.0018245967871751165</v>
+        <v>0.0018245967875374165</v>
       </c>
       <c r="M63" s="1">
-        <v>0.9282994021747486</v>
+        <v>0.92829940217511098</v>
       </c>
       <c r="N63" s="1">
         <v>0.81959354877471924</v>
@@ -3852,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G64" s="1">
         <v>-0.0017523671022848001</v>
@@ -3861,7 +3861,7 @@
         <v>0.09782399982213974</v>
       </c>
       <c r="I64" s="1">
-        <v>0.61006330090756156</v>
+        <v>0.6100633008901929</v>
       </c>
       <c r="J64" s="1">
         <v>1</v>
@@ -3870,13 +3870,13 @@
         <v>-0.12013750523328781</v>
       </c>
       <c r="L64" s="1">
-        <v>0.0029837561110548998</v>
+        <v>0.0029837561114171999</v>
       </c>
       <c r="M64" s="1">
-        <v>0.88284624742073137</v>
+        <v>0.88284624742109363</v>
       </c>
       <c r="N64" s="1">
-        <v>0.69101873932169333</v>
+        <v>0.6910187393017363</v>
       </c>
     </row>
     <row r="65">
@@ -3896,7 +3896,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G65" s="1">
         <v>-0.0017523671022848001</v>
@@ -3905,7 +3905,7 @@
         <v>0.084419429302215576</v>
       </c>
       <c r="I65" s="1">
-        <v>0.66323720597707947</v>
+        <v>0.66323720595971081</v>
       </c>
       <c r="J65" s="1">
         <v>1</v>
@@ -3914,13 +3914,13 @@
         <v>-0.10369761288166046</v>
       </c>
       <c r="L65" s="1">
-        <v>0.0025749273502184001</v>
+        <v>0.0025749273505807002</v>
       </c>
       <c r="M65" s="1">
-        <v>0.89887731109884517</v>
+        <v>0.89887731109920754</v>
       </c>
       <c r="N65" s="1">
-        <v>0.73785064745520812</v>
+        <v>0.73785064743558804</v>
       </c>
     </row>
     <row r="66">
@@ -3940,7 +3940,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G66" s="1">
         <v>-0.0017523671022848001</v>
@@ -3949,7 +3949,7 @@
         <v>0.078249067068099976</v>
       </c>
       <c r="I66" s="1">
-        <v>0.68771408291384117</v>
+        <v>0.68771408289647251</v>
       </c>
       <c r="J66" s="1">
         <v>1</v>
@@ -3958,13 +3958,13 @@
         <v>-0.096130043268203735</v>
       </c>
       <c r="L66" s="1">
-        <v>0.0023867363333253998</v>
+        <v>0.0023867363336876998</v>
       </c>
       <c r="M66" s="1">
-        <v>0.90625668961734207</v>
+        <v>0.90625668961770434</v>
       </c>
       <c r="N66" s="1">
-        <v>0.75885131750500146</v>
+        <v>0.75885131748553281</v>
       </c>
     </row>
     <row r="67">
@@ -3984,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G67" s="1">
         <v>-0.0017523671022848001</v>
@@ -3993,7 +3993,7 @@
         <v>0.075483039021492004</v>
       </c>
       <c r="I67" s="1">
-        <v>0.69868647602342438</v>
+        <v>0.69868647600605571</v>
       </c>
       <c r="J67" s="1">
         <v>1</v>
@@ -4002,13 +4002,13 @@
         <v>-0.09273768961429596</v>
       </c>
       <c r="L67" s="1">
-        <v>0.002302374842994</v>
+        <v>0.0023023748433563</v>
       </c>
       <c r="M67" s="1">
-        <v>0.9095646868842544</v>
+        <v>0.90956468688461667</v>
       </c>
       <c r="N67" s="1">
-        <v>0.76815479547342513</v>
+        <v>0.76815479545402354</v>
       </c>
     </row>
     <row r="68">
@@ -4028,7 +4028,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G68" s="1">
         <v>-0.0017523671022848001</v>
@@ -4037,7 +4037,7 @@
         <v>0.071014851331710815</v>
       </c>
       <c r="I68" s="1">
-        <v>0.71641111104659705</v>
+        <v>0.71641111102922839</v>
       </c>
       <c r="J68" s="1">
         <v>1</v>
@@ -4046,13 +4046,13 @@
         <v>-0.087257720530033112</v>
       </c>
       <c r="L68" s="1">
-        <v>0.0021660985893817999</v>
+        <v>0.0021660985897440999</v>
       </c>
       <c r="M68" s="1">
-        <v>0.91490837477695897</v>
+        <v>0.91490837477732134</v>
       </c>
       <c r="N68" s="1">
-        <v>0.78304137419361519</v>
+        <v>0.78304137417432096</v>
       </c>
     </row>
     <row r="69">
@@ -4072,7 +4072,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G69" s="1">
         <v>-0.0017523671022848001</v>
@@ -4081,7 +4081,7 @@
         <v>0.068674370646476746</v>
       </c>
       <c r="I69" s="1">
-        <v>0.72569544367778283</v>
+        <v>0.72569544366041416</v>
       </c>
       <c r="J69" s="1">
         <v>1</v>
@@ -4090,13 +4090,13 @@
         <v>-0.084387265145778656</v>
       </c>
       <c r="L69" s="1">
-        <v>0.0020947157898707001</v>
+        <v>0.0020947157902330002</v>
       </c>
       <c r="M69" s="1">
-        <v>0.91770744938742344</v>
+        <v>0.9177074493877857</v>
       </c>
       <c r="N69" s="1">
-        <v>0.79076991710396372</v>
+        <v>0.79076991708472544</v>
       </c>
     </row>
     <row r="70">
@@ -4116,7 +4116,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G70" s="1">
         <v>-0.0017523671022848001</v>
@@ -4125,7 +4125,7 @@
         <v>0.062716774642467499</v>
       </c>
       <c r="I70" s="1">
-        <v>0.74932829037534643</v>
+        <v>0.74932829035797777</v>
       </c>
       <c r="J70" s="1">
         <v>1</v>
@@ -4134,13 +4134,13 @@
         <v>-0.07708064466714859</v>
       </c>
       <c r="L70" s="1">
-        <v>0.0019130141183878</v>
+        <v>0.0019130141187501</v>
       </c>
       <c r="M70" s="1">
-        <v>0.9248323665776963</v>
+        <v>0.92483236657805856</v>
       </c>
       <c r="N70" s="1">
-        <v>0.81023147270267437</v>
+        <v>0.81023147268357665</v>
       </c>
     </row>
     <row r="71">
@@ -4160,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G71" s="1">
         <v>-0.0017523671022848001</v>
@@ -4169,7 +4169,7 @@
         <v>0.05952521413564682</v>
       </c>
       <c r="I71" s="1">
-        <v>0.7619887439633265</v>
+        <v>0.76198874394595784</v>
       </c>
       <c r="J71" s="1">
         <v>1</v>
@@ -4178,13 +4178,13 @@
         <v>-0.073166385293006897</v>
       </c>
       <c r="L71" s="1">
-        <v>0.0018156739372362</v>
+        <v>0.0018156739375985</v>
       </c>
       <c r="M71" s="1">
-        <v>0.9286492865010566</v>
+        <v>0.92864928650141887</v>
       </c>
       <c r="N71" s="1">
-        <v>0.82053446337565195</v>
+        <v>0.82053446335662872</v>
       </c>
     </row>
     <row r="72">
@@ -4204,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G72" s="1">
         <v>-0.0017523671022848001</v>
@@ -4213,7 +4213,7 @@
         <v>0.042077984660863876</v>
       </c>
       <c r="I72" s="1">
-        <v>0.83119922357761977</v>
+        <v>0.831199223560251</v>
       </c>
       <c r="J72" s="1">
         <v>1</v>
@@ -4222,13 +4222,13 @@
         <v>-0.051768433302640915</v>
       </c>
       <c r="L72" s="1">
-        <v>0.0012835476136076999</v>
+        <v>0.00128354761397</v>
       </c>
       <c r="M72" s="1">
-        <v>0.94951511541542721</v>
+        <v>0.94951511541578948</v>
       </c>
       <c r="N72" s="1">
-        <v>0.87539335612783531</v>
+        <v>0.8753933561092091</v>
       </c>
     </row>
     <row r="73">
@@ -4248,7 +4248,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G73" s="1">
         <v>-0.0017523671022848001</v>
@@ -4257,7 +4257,7 @@
         <v>0.034843768924474716</v>
       </c>
       <c r="I73" s="1">
-        <v>0.85989625171037531</v>
+        <v>0.85989625169300665</v>
       </c>
       <c r="J73" s="1">
         <v>1</v>
@@ -4266,13 +4266,13 @@
         <v>-0.042896110564470291</v>
       </c>
       <c r="L73" s="1">
-        <v>0.0010629098696641999</v>
+        <v>0.0010629098700265</v>
       </c>
       <c r="M73" s="1">
-        <v>0.958166800575044</v>
+        <v>0.95816680057540637</v>
       </c>
       <c r="N73" s="1">
-        <v>0.89743899621058509</v>
+        <v>0.89743899619211864</v>
       </c>
     </row>
     <row r="74">
@@ -4292,7 +4292,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G74" s="1">
         <v>-0.0017523671022848001</v>
@@ -4301,7 +4301,7 @@
         <v>0.034099072217941284</v>
       </c>
       <c r="I74" s="1">
-        <v>0.86285035754757056</v>
+        <v>0.86285035753020189</v>
       </c>
       <c r="J74" s="1">
         <v>1</v>
@@ -4310,13 +4310,13 @@
         <v>-0.041982781141996384</v>
       </c>
       <c r="L74" s="1">
-        <v>0.0010401971607287999</v>
+        <v>0.0010401971610911</v>
       </c>
       <c r="M74" s="1">
-        <v>0.95905741522382804</v>
+        <v>0.9590574152241903</v>
       </c>
       <c r="N74" s="1">
-        <v>0.89968582052639223</v>
+        <v>0.89968582050794221</v>
       </c>
     </row>
     <row r="75">
@@ -4336,7 +4336,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G75" s="1">
         <v>-0.0017523671022848001</v>
@@ -4345,7 +4345,7 @@
         <v>0.0088857021182775498</v>
       </c>
       <c r="I75" s="1">
-        <v>0.96286794089261607</v>
+        <v>0.96286794087524741</v>
       </c>
       <c r="J75" s="1">
         <v>1</v>
@@ -4354,13 +4354,13 @@
         <v>-0.011060127057135105</v>
       </c>
       <c r="L75" s="1">
-        <v>0.00027120972963149998</v>
+        <v>0.00027120972999380001</v>
       </c>
       <c r="M75" s="1">
-        <v>0.98921108261837576</v>
+        <v>0.98921108261873814</v>
       </c>
       <c r="N75" s="1">
-        <v>0.97336954448990687</v>
+        <v>0.9733695444719922</v>
       </c>
     </row>
     <row r="76">
@@ -4380,7 +4380,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G76" s="1">
         <v>-0.0017523671022848001</v>
@@ -4389,7 +4389,7 @@
         <v>0.097375713288784027</v>
       </c>
       <c r="I76" s="1">
-        <v>0.6118415815233611</v>
+        <v>0.61184158150599244</v>
       </c>
       <c r="J76" s="1">
         <v>1</v>
@@ -4398,13 +4398,13 @@
         <v>-0.11958771198987961</v>
       </c>
       <c r="L76" s="1">
-        <v>0.0029700837606863001</v>
+        <v>0.0029700837610486001</v>
       </c>
       <c r="M76" s="1">
-        <v>0.88338236997468267</v>
+        <v>0.88338236997504494</v>
       </c>
       <c r="N76" s="1">
-        <v>0.69261239789163576</v>
+        <v>0.69261239787169016</v>
       </c>
     </row>
     <row r="77">
@@ -4424,7 +4424,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G77" s="1">
         <v>-0.0017523671022848001</v>
@@ -4433,7 +4433,7 @@
         <v>0.092504724860191345</v>
       </c>
       <c r="I77" s="1">
-        <v>0.63116405688752897</v>
+        <v>0.63116405687016031</v>
       </c>
       <c r="J77" s="1">
         <v>1</v>
@@ -4442,13 +4442,13 @@
         <v>-0.11361373960971832</v>
       </c>
       <c r="L77" s="1">
-        <v>0.0028215224758022998</v>
+        <v>0.0028215224761645999</v>
       </c>
       <c r="M77" s="1">
-        <v>0.88920778062633188</v>
+        <v>0.88920778062669426</v>
       </c>
       <c r="N77" s="1">
-        <v>0.70980491920904643</v>
+        <v>0.70980491918922439</v>
       </c>
     </row>
     <row r="78">
@@ -4468,7 +4468,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G78" s="1">
         <v>-0.0017523671022848001</v>
@@ -4477,7 +4477,7 @@
         <v>0.074419185519218445</v>
       </c>
       <c r="I78" s="1">
-        <v>0.70290662721941799</v>
+        <v>0.70290662720204933</v>
       </c>
       <c r="J78" s="1">
         <v>1</v>
@@ -4486,13 +4486,13 @@
         <v>-0.091432936489582062</v>
       </c>
       <c r="L78" s="1">
-        <v>0.0022699281159435001</v>
+        <v>0.0022699281163058001</v>
       </c>
       <c r="M78" s="1">
-        <v>0.91083699352537462</v>
+        <v>0.91083699352573688</v>
       </c>
       <c r="N78" s="1">
-        <v>0.77171506231738929</v>
+        <v>0.77171506229801345</v>
       </c>
     </row>
     <row r="79">
@@ -4512,7 +4512,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G79" s="1">
         <v>-0.0017523671022848001</v>
@@ -4521,7 +4521,7 @@
         <v>0.071227617561817169</v>
       </c>
       <c r="I79" s="1">
-        <v>0.71556708080739828</v>
+        <v>0.71556708079002962</v>
       </c>
       <c r="J79" s="1">
         <v>1</v>
@@ -4530,13 +4530,13 @@
         <v>-0.087518677115440369</v>
       </c>
       <c r="L79" s="1">
-        <v>0.002172587934792</v>
+        <v>0.0021725879351541999</v>
       </c>
       <c r="M79" s="1">
-        <v>0.91465391344873503</v>
+        <v>0.91465391344909719</v>
       </c>
       <c r="N79" s="1">
-        <v>0.78233643379857987</v>
+        <v>0.78233643377928075</v>
       </c>
     </row>
     <row r="80">
@@ -4556,7 +4556,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G80" s="1">
         <v>-0.0017523671022848001</v>
@@ -4565,7 +4565,7 @@
         <v>0.06675942987203598</v>
       </c>
       <c r="I80" s="1">
-        <v>0.73329171583057107</v>
+        <v>0.73329171581320241</v>
       </c>
       <c r="J80" s="1">
         <v>1</v>
@@ -4574,13 +4574,13 @@
         <v>-0.082038708031177521</v>
       </c>
       <c r="L80" s="1">
-        <v>0.0020363116811797999</v>
+        <v>0.0020363116815421</v>
       </c>
       <c r="M80" s="1">
-        <v>0.9199976013414396</v>
+        <v>0.91999760134180186</v>
       </c>
       <c r="N80" s="1">
-        <v>0.79705829097963465</v>
+        <v>0.79705829096044178</v>
       </c>
     </row>
     <row r="81">
@@ -4600,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="1">
-        <v>-0.00021502111970549999</v>
+        <v>-0.0002150211370742</v>
       </c>
       <c r="G81" s="1">
         <v>-0.0017523671022848001</v>
@@ -4609,7 +4609,7 @@
         <v>0.014141147024929523</v>
       </c>
       <c r="I81" s="1">
-        <v>0.94202039398440818</v>
+        <v>0.94202039396703952</v>
       </c>
       <c r="J81" s="1">
         <v>1</v>
@@ -4618,13 +4618,13 @@
         <v>-0.01750560849905014</v>
       </c>
       <c r="L81" s="1">
-        <v>0.00043149656126110001</v>
+        <v>0.00043149656162339999</v>
       </c>
       <c r="M81" s="1">
-        <v>0.98292588781124213</v>
+        <v>0.9829258878116045</v>
       </c>
       <c r="N81" s="1">
-        <v>0.95838394905039948</v>
+        <v>0.95838394903237578</v>
       </c>
     </row>
     <row r="82">

</xml_diff>